<commit_message>
small update API DOCS
</commit_message>
<xml_diff>
--- a/API DOC_1차 수정본.xlsx
+++ b/API DOC_1차 수정본.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>path</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -183,10 +183,6 @@
   </si>
   <si>
     <t>영화 추천</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>정해주세요</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -287,6 +283,42 @@
   </si>
   <si>
     <t>{ "detail" : "Successfully logged out." }</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;int:articlePk&gt;/comments/</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>back</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>todo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>recommendations/</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -391,7 +423,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -539,6 +571,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -557,7 +598,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -629,6 +670,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="4" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -948,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -963,15 +1013,15 @@
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
@@ -982,18 +1032,21 @@
         <v>1</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>41</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -1002,16 +1055,19 @@
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8" t="s">
         <v>4</v>
@@ -1023,13 +1079,16 @@
         <v>31</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
         <v>5</v>
@@ -1038,16 +1097,19 @@
         <v>7</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="G6" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="27" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8" t="s">
         <v>9</v>
@@ -1056,16 +1118,19 @@
         <v>8</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>10</v>
       </c>
@@ -1079,13 +1144,16 @@
         <v>31</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
         <v>11</v>
@@ -1094,16 +1162,19 @@
         <v>8</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
         <v>12</v>
@@ -1112,16 +1183,19 @@
         <v>7</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
         <v>13</v>
@@ -1130,16 +1204,19 @@
         <v>15</v>
       </c>
       <c r="D11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="8" t="s">
         <v>13</v>
@@ -1148,7 +1225,7 @@
         <v>23</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>31</v>
@@ -1156,11 +1233,14 @@
       <c r="F12" s="10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="13" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>8</v>
@@ -1169,13 +1249,16 @@
         <v>31</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
@@ -1189,13 +1272,16 @@
         <v>31</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="14" t="s">
         <v>31</v>
@@ -1204,16 +1290,19 @@
         <v>7</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8" t="s">
         <v>32</v>
@@ -1222,16 +1311,19 @@
         <v>15</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="8" t="s">
         <v>32</v>
@@ -1240,7 +1332,7 @@
         <v>23</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>31</v>
@@ -1248,26 +1340,32 @@
       <c r="F17" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="8" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="8" t="s">
         <v>36</v>
@@ -1276,16 +1374,19 @@
         <v>15</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
         <v>36</v>
@@ -1294,7 +1395,7 @@
         <v>23</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>31</v>
@@ -1302,8 +1403,11 @@
       <c r="F20" s="18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
     </row>
   </sheetData>

</xml_diff>